<commit_message>
provider test cases added
</commit_message>
<xml_diff>
--- a/ezugi_staging_backend_framework_automation/testscriptdata/TestScriptData.xlsx
+++ b/ezugi_staging_backend_framework_automation/testscriptdata/TestScriptData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12240"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="ezugi" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>Main data</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>launchToken</t>
-  </si>
-  <si>
-    <t>ecc099a3-029a-464f-a5ea-3e2912db6b03</t>
   </si>
   <si>
     <t>transactionalToken</t>
@@ -802,7 +799,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1172,15 +1169,15 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="9.57407407407407" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="21.712962962963" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="54.5740740740741" collapsed="true"/>
-    <col min="4" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="9.57142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7142857142857" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5714285714286" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1307,10 +1304,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1318,10 +1315,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1329,10 +1326,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1340,7 +1337,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>12</v>
@@ -1351,10 +1348,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1362,10 +1359,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1373,10 +1370,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
         <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Response validation class added
</commit_message>
<xml_diff>
--- a/ezugi_staging_backend_framework_automation/testscriptdata/TestScriptData.xlsx
+++ b/ezugi_staging_backend_framework_automation/testscriptdata/TestScriptData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>Main data</t>
   </si>
@@ -147,13 +147,7 @@
     <t>player token / platform token</t>
   </si>
   <si>
-    <t>1000002</t>
-  </si>
-  <si>
-    <t>betvita</t>
-  </si>
-  <si>
-    <t>859e7645-a721-4649-b663-19de06fa5eca-1731486168660</t>
+    <t>c0987b11-c5d6-4746-a763-ac07fde2e4b8-1731498207823</t>
   </si>
   <si>
     <t>authentication API</t>
@@ -165,6 +159,9 @@
     <t>authToken</t>
   </si>
   <si>
+    <t>1de226a6-f79f-4d42-9b51-910526259109</t>
+  </si>
+  <si>
     <t>Debit API</t>
   </si>
   <si>
@@ -199,6 +196,12 @@
   </si>
   <si>
     <t>104</t>
+  </si>
+  <si>
+    <t>d628b6d5-cfe0-41d1-89c4-d4964e76995c</t>
+  </si>
+  <si>
+    <t>2712dd32-8386-4610-b361-ebb1329f0aa5</t>
   </si>
 </sst>
 </file>
@@ -930,7 +933,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1332,10 +1335,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="9.57142857142857" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.7142857142857" style="16" customWidth="1"/>
-    <col min="3" max="3" width="54.5714285714286" style="16" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="16"/>
+    <col min="1" max="1" customWidth="true" style="16" width="9.57142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="21.7142857142857" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="16" width="54.5714285714286" collapsed="true"/>
+    <col min="4" max="16384" style="16" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1551,20 +1554,21 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.8571428571429" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="22.7142857142857" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.2857142857143" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1428571428571" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.8571428571429" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1428571428571" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.2857142857143" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="9" width="16.4285714285714" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="22.8571428571429" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="40.1428571428571" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="16.1428571428571" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="21.1428571428571" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="49.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="17.5714285714286" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="20.2857142857143" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="8.85714285714286" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="16.4285714285714" collapsed="true"/>
+    <col min="10" max="16384" customWidth="true" style="1" width="22.8571428571429" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1595,16 +1599,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="27" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>40</v>
+      <c r="C3" t="s">
+        <v>19</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>8</v>
@@ -1612,7 +1616,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1622,10 +1626,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1633,8 +1637,12 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7"/>
-      <c r="B7" s="6"/>
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1642,7 +1650,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1655,7 +1663,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>31</v>
@@ -1664,13 +1672,13 @@
         <v>24</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>28</v>
@@ -1692,7 +1700,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="11" t="s">
@@ -1701,7 +1709,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1716,29 +1724,29 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>

</xml_diff>

<commit_message>
added balance method in BaseAPiClass
</commit_message>
<xml_diff>
--- a/ezugi_staging_backend_framework_automation/testscriptdata/TestScriptData.xlsx
+++ b/ezugi_staging_backend_framework_automation/testscriptdata/TestScriptData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="8940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ezugi" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
   <si>
     <t>Main data</t>
   </si>
@@ -147,7 +147,7 @@
     <t>player token / platform token</t>
   </si>
   <si>
-    <t>c0987b11-c5d6-4746-a763-ac07fde2e4b8-1731498207823</t>
+    <t>6a4cca3e-4758-48ec-b291-23037272cd00-1731587810166</t>
   </si>
   <si>
     <t>authentication API</t>
@@ -159,7 +159,10 @@
     <t>authToken</t>
   </si>
   <si>
-    <t>1de226a6-f79f-4d42-9b51-910526259109</t>
+    <t>c1222e7d-9c68-4b34-aeda-63333762e3c4</t>
+  </si>
+  <si>
+    <t>2712dd32-8386-4610-b361-ebb1329f0aa5</t>
   </si>
   <si>
     <t>Debit API</t>
@@ -198,10 +201,28 @@
     <t>104</t>
   </si>
   <si>
-    <t>d628b6d5-cfe0-41d1-89c4-d4964e76995c</t>
-  </si>
-  <si>
-    <t>2712dd32-8386-4610-b361-ebb1329f0aa5</t>
+    <t>2dae7ec8-4869-4d42-8207-83c4f3fcbda1</t>
+  </si>
+  <si>
+    <t>b0ab4f72-0179-41d3-a89a-58c2a58108f1</t>
+  </si>
+  <si>
+    <t>3c7bd6dc-d6b8-4c1c-9134-ad84be52e39f</t>
+  </si>
+  <si>
+    <t>e1f09830-ec87-46f7-bc59-23e7039f129c</t>
+  </si>
+  <si>
+    <t>e575c477-0b75-48a0-a86c-d175b8ec006a</t>
+  </si>
+  <si>
+    <t>ae8246a3-ecd4-4433-8051-223e20f0a794</t>
+  </si>
+  <si>
+    <t>3ab3efae-4a49-4f81-b766-2adb9c828045</t>
+  </si>
+  <si>
+    <t>53a967ec-645a-4e41-9f50-ce78ff0dc2a0</t>
   </si>
 </sst>
 </file>
@@ -1597,7 +1618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" ht="30" spans="1:5">
       <c r="A3" s="27" t="s">
         <v>6</v>
       </c>
@@ -1638,10 +1659,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1650,7 +1671,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1663,7 +1684,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>31</v>
@@ -1672,13 +1693,13 @@
         <v>24</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>28</v>
@@ -1700,7 +1721,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="11" t="s">
@@ -1709,7 +1730,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1724,29 +1745,29 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>

</xml_diff>